<commit_message>
updated .py and excel
</commit_message>
<xml_diff>
--- a/Race_Gender_Breakdown.xlsx
+++ b/Race_Gender_Breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/as822/Documents/GitHub/FLXSUS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91697EF2-C5F9-8B43-8543-D7FA4821ACCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3F8530-6819-044B-A669-2833288E954A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5480" windowWidth="34400" windowHeight="28300" xr2:uid="{101D7EF5-ACAD-E84A-BEB6-A21BB2D31C28}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{101D7EF5-ACAD-E84A-BEB6-A21BB2D31C28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -702,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA2A70C-FCDE-6F48-94D9-0CF2A215B8C8}">
   <dimension ref="A1:AF511"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O64" zoomScale="116" workbookViewId="0">
-      <selection activeCell="W92" sqref="W92"/>
+    <sheetView tabSelected="1" topLeftCell="X65" zoomScale="116" workbookViewId="0">
+      <selection activeCell="AF87" sqref="AF87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2360,7 +2360,7 @@
         <v>16</v>
       </c>
       <c r="R28">
-        <f>R14</f>
+        <f t="shared" ref="R28:R35" si="6">R14</f>
         <v>9</v>
       </c>
     </row>
@@ -2411,7 +2411,7 @@
         <v>17</v>
       </c>
       <c r="R29">
-        <f>R15</f>
+        <f t="shared" si="6"/>
         <v>361</v>
       </c>
     </row>
@@ -2462,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="R30">
-        <f>R16</f>
+        <f t="shared" si="6"/>
         <v>71</v>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
         <v>19</v>
       </c>
       <c r="R31">
-        <f>R17</f>
+        <f t="shared" si="6"/>
         <v>116</v>
       </c>
     </row>
@@ -2564,7 +2564,7 @@
         <v>20</v>
       </c>
       <c r="R32">
-        <f>R18</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -2615,7 +2615,7 @@
         <v>21</v>
       </c>
       <c r="R33">
-        <f>R19</f>
+        <f t="shared" si="6"/>
         <v>931</v>
       </c>
     </row>
@@ -2666,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="R34">
-        <f>R20</f>
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
         <v>22</v>
       </c>
       <c r="R35">
-        <f>R21</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4147,19 +4147,19 @@
         <v>263</v>
       </c>
       <c r="S61">
-        <f t="shared" ref="S61:V61" si="6">COUNTIF(B:B,TRUE)</f>
+        <f t="shared" ref="S61:V61" si="7">COUNTIF(B:B,TRUE)</f>
         <v>123</v>
       </c>
       <c r="T61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>282</v>
       </c>
       <c r="U61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>152</v>
       </c>
       <c r="V61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>83</v>
       </c>
     </row>
@@ -4995,19 +4995,19 @@
         <v>25</v>
       </c>
       <c r="S76">
-        <f t="shared" ref="S76:V76" si="7">S58+S60</f>
+        <f t="shared" ref="S76:V76" si="8">S58+S60</f>
         <v>14</v>
       </c>
       <c r="T76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="U76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="V76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="W76" s="9" t="s">
@@ -5341,23 +5341,23 @@
         <v>141 (53.6%)</v>
       </c>
       <c r="AB81" t="str">
-        <f t="shared" ref="AB81:AF81" si="8">CONCATENATE(S81," (",TEXT(S92,"0.0%"),")")</f>
+        <f t="shared" ref="AB81:AF81" si="9">CONCATENATE(S81," (",TEXT(S92,"0.0%"),")")</f>
         <v>64 (52.0%)</v>
       </c>
       <c r="AC81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>148 (52.5%)</v>
       </c>
       <c r="AD81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>83 (54.6%)</v>
       </c>
       <c r="AE81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>47 (56.6%)</v>
       </c>
       <c r="AF81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>71 (4.5%)</v>
       </c>
     </row>
@@ -5430,27 +5430,27 @@
         <v>33</v>
       </c>
       <c r="AA82" t="str">
-        <f t="shared" ref="AA82:AF82" si="9">CONCATENATE(R82," (",TEXT(R93,"0.0%"),")")</f>
+        <f t="shared" ref="AA82:AF82" si="10">CONCATENATE(R82," (",TEXT(R93,"0.0%"),")")</f>
         <v>63 (24.0%)</v>
       </c>
       <c r="AB82" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>33 (26.8%)</v>
       </c>
       <c r="AC82" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>43 (15.2%)</v>
       </c>
       <c r="AD82" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>21 (13.8%)</v>
       </c>
       <c r="AE82" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12 (14.5%)</v>
       </c>
       <c r="AF82" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>931 (59.4%)</v>
       </c>
     </row>
@@ -5523,27 +5523,27 @@
         <v>34</v>
       </c>
       <c r="AA83" t="str">
-        <f t="shared" ref="AA83:AF83" si="10">CONCATENATE(R83," (",TEXT(R94,"0.0%"),")")</f>
+        <f t="shared" ref="AA83:AF83" si="11">CONCATENATE(R83," (",TEXT(R94,"0.0%"),")")</f>
         <v>94 (35.7%)</v>
       </c>
       <c r="AB83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>48 (39.0%)</v>
       </c>
       <c r="AC83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>93 (33.0%)</v>
       </c>
       <c r="AD83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>40 (26.3%)</v>
       </c>
       <c r="AE83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>18 (21.7%)</v>
       </c>
       <c r="AF83" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>361 (23.0%)</v>
       </c>
     </row>
@@ -5616,27 +5616,27 @@
         <v>16</v>
       </c>
       <c r="AA84" t="str">
-        <f t="shared" ref="AA84:AF84" si="11">CONCATENATE(R84," (",TEXT(R95,"0.0%"),")")</f>
+        <f t="shared" ref="AA84:AF84" si="12">CONCATENATE(R84," (",TEXT(R95,"0.0%"),")")</f>
         <v>4 (1.5%)</v>
       </c>
       <c r="AB84" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2 (1.6%)</v>
       </c>
       <c r="AC84" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6 (2.1%)</v>
       </c>
       <c r="AD84" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3 (2.0%)</v>
       </c>
       <c r="AE84" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2 (2.4%)</v>
       </c>
       <c r="AF84" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9 (0.6%)</v>
       </c>
     </row>
@@ -5709,27 +5709,27 @@
         <v>36</v>
       </c>
       <c r="AA85" t="str">
-        <f t="shared" ref="AA85:AF85" si="12">CONCATENATE(R85," (",TEXT(R96,"0.0%"),")")</f>
+        <f t="shared" ref="AA85:AF85" si="13">CONCATENATE(R85," (",TEXT(R96,"0.0%"),")")</f>
         <v>25 (9.5%)</v>
       </c>
       <c r="AB85" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>14 (11.4%)</v>
       </c>
       <c r="AC85" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37 (13.1%)</v>
       </c>
       <c r="AD85" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22 (14.5%)</v>
       </c>
       <c r="AE85" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12 (14.5%)</v>
       </c>
       <c r="AF85" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>69 (4.4%)</v>
       </c>
     </row>
@@ -5802,27 +5802,27 @@
         <v>19</v>
       </c>
       <c r="AA86" t="str">
-        <f t="shared" ref="AA86:AF86" si="13">CONCATENATE(R86," (",TEXT(R97,"0.0%"),")")</f>
+        <f t="shared" ref="AA86:AF86" si="14">CONCATENATE(R86," (",TEXT(R97,"0.0%"),")")</f>
         <v>71 (27.0%)</v>
       </c>
       <c r="AB86" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>37 (30.1%)</v>
       </c>
       <c r="AC86" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>62 (22.0%)</v>
       </c>
       <c r="AD86" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>38 (25.0%)</v>
       </c>
       <c r="AE86" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>19 (22.9%)</v>
       </c>
       <c r="AF86" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>116 (7.4%)</v>
       </c>
     </row>
@@ -5899,23 +5899,23 @@
         <v>263</v>
       </c>
       <c r="AB87">
-        <f t="shared" ref="AB87:AF87" si="14">S87</f>
+        <f t="shared" ref="AB87:AF87" si="15">S87</f>
         <v>123</v>
       </c>
       <c r="AC87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>282</v>
       </c>
       <c r="AD87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>152</v>
       </c>
       <c r="AE87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>83</v>
       </c>
       <c r="AF87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1567</v>
       </c>
     </row>
@@ -6167,23 +6167,23 @@
         <v>0.53612167300380231</v>
       </c>
       <c r="S92">
-        <f t="shared" ref="S92:W92" si="15">S81/S$87</f>
+        <f t="shared" ref="S92:W92" si="16">S81/S$87</f>
         <v>0.52032520325203258</v>
       </c>
       <c r="T92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.52482269503546097</v>
       </c>
       <c r="U92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.54605263157894735</v>
       </c>
       <c r="V92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.5662650602409639</v>
       </c>
       <c r="W92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.530950861518826E-2</v>
       </c>
     </row>
@@ -6234,27 +6234,27 @@
         <v>33</v>
       </c>
       <c r="R93">
-        <f t="shared" ref="R93:W93" si="16">R82/R$87</f>
+        <f t="shared" ref="R93:W93" si="17">R82/R$87</f>
         <v>0.23954372623574144</v>
       </c>
       <c r="S93">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.26829268292682928</v>
       </c>
       <c r="T93">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.1524822695035461</v>
       </c>
       <c r="U93">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.13815789473684212</v>
       </c>
       <c r="V93">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.14457831325301204</v>
       </c>
       <c r="W93">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.59412890874282065</v>
       </c>
     </row>
@@ -6305,27 +6305,27 @@
         <v>34</v>
       </c>
       <c r="R94">
-        <f t="shared" ref="R94:W94" si="17">R83/R$87</f>
+        <f t="shared" ref="R94:W94" si="18">R83/R$87</f>
         <v>0.35741444866920152</v>
       </c>
       <c r="S94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.3902439024390244</v>
       </c>
       <c r="T94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.32978723404255317</v>
       </c>
       <c r="U94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.26315789473684209</v>
       </c>
       <c r="V94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.21686746987951808</v>
       </c>
       <c r="W94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.23037651563497127</v>
       </c>
     </row>
@@ -6376,27 +6376,27 @@
         <v>16</v>
       </c>
       <c r="R95">
-        <f t="shared" ref="R95:W95" si="18">R84/R$87</f>
+        <f t="shared" ref="R95:W95" si="19">R84/R$87</f>
         <v>1.5209125475285171E-2</v>
       </c>
       <c r="S95">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.6260162601626018E-2</v>
       </c>
       <c r="T95">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="U95">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.9736842105263157E-2</v>
       </c>
       <c r="V95">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2.4096385542168676E-2</v>
       </c>
       <c r="W95">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5.7434588385449903E-3</v>
       </c>
     </row>
@@ -6447,27 +6447,27 @@
         <v>36</v>
       </c>
       <c r="R96">
-        <f t="shared" ref="R96:W96" si="19">R85/R$87</f>
+        <f t="shared" ref="R96:W96" si="20">R85/R$87</f>
         <v>9.5057034220532313E-2</v>
       </c>
       <c r="S96">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.11382113821138211</v>
       </c>
       <c r="T96">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.13120567375886524</v>
       </c>
       <c r="U96">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.14473684210526316</v>
       </c>
       <c r="V96">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.14457831325301204</v>
       </c>
       <c r="W96">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>4.4033184428844928E-2</v>
       </c>
     </row>
@@ -6518,27 +6518,27 @@
         <v>19</v>
       </c>
       <c r="R97">
-        <f t="shared" ref="R97:W97" si="20">R86/R$87</f>
+        <f t="shared" ref="R97:W97" si="21">R86/R$87</f>
         <v>0.26996197718631176</v>
       </c>
       <c r="S97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.30081300813008133</v>
       </c>
       <c r="T97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.21985815602836881</v>
       </c>
       <c r="U97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.25</v>
       </c>
       <c r="V97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.2289156626506024</v>
       </c>
       <c r="W97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>7.4026802807913211E-2</v>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
         <v>931</v>
       </c>
       <c r="T104">
-        <f t="shared" ref="T104:T109" si="21">S104+R104</f>
+        <f t="shared" ref="T104:T109" si="22">S104+R104</f>
         <v>943</v>
       </c>
     </row>
@@ -6988,7 +6988,7 @@
         <v>361</v>
       </c>
       <c r="T105">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>379</v>
       </c>
     </row>
@@ -7045,7 +7045,7 @@
         <v>9</v>
       </c>
       <c r="T106">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>11</v>
       </c>
     </row>
@@ -7102,7 +7102,7 @@
         <v>69</v>
       </c>
       <c r="T107">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>81</v>
       </c>
     </row>
@@ -7159,7 +7159,7 @@
         <v>116</v>
       </c>
       <c r="T108">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>135</v>
       </c>
     </row>
@@ -7216,7 +7216,7 @@
         <v>1567</v>
       </c>
       <c r="T109">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1650</v>
       </c>
     </row>
@@ -7423,7 +7423,7 @@
         <v>47.435757575757577</v>
       </c>
       <c r="S113">
-        <f t="shared" ref="S113:S117" si="22">SUM((S$109*$T104)/$T$109)</f>
+        <f t="shared" ref="S113:S117" si="23">SUM((S$109*$T104)/$T$109)</f>
         <v>895.56424242424248</v>
       </c>
     </row>
@@ -7474,11 +7474,11 @@
         <v>34</v>
       </c>
       <c r="R114">
-        <f t="shared" ref="R114" si="23">SUM((R$109*$T105)/$T$109)</f>
+        <f t="shared" ref="R114" si="24">SUM((R$109*$T105)/$T$109)</f>
         <v>19.064848484848486</v>
       </c>
       <c r="S114">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>359.93515151515152</v>
       </c>
     </row>
@@ -7529,11 +7529,11 @@
         <v>16</v>
       </c>
       <c r="R115">
-        <f t="shared" ref="R115" si="24">SUM((R$109*$T106)/$T$109)</f>
+        <f t="shared" ref="R115" si="25">SUM((R$109*$T106)/$T$109)</f>
         <v>0.55333333333333334</v>
       </c>
       <c r="S115">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>10.446666666666667</v>
       </c>
     </row>
@@ -7584,11 +7584,11 @@
         <v>36</v>
       </c>
       <c r="R116">
-        <f t="shared" ref="R116" si="25">SUM((R$109*$T107)/$T$109)</f>
+        <f t="shared" ref="R116" si="26">SUM((R$109*$T107)/$T$109)</f>
         <v>4.0745454545454542</v>
       </c>
       <c r="S116">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>76.925454545454542</v>
       </c>
     </row>
@@ -7639,11 +7639,11 @@
         <v>19</v>
       </c>
       <c r="R117">
-        <f t="shared" ref="R117" si="26">SUM((R$109*$T108)/$T$109)</f>
+        <f t="shared" ref="R117" si="27">SUM((R$109*$T108)/$T$109)</f>
         <v>6.790909090909091</v>
       </c>
       <c r="S117">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>128.20909090909092</v>
       </c>
     </row>
@@ -8080,23 +8080,23 @@
         <v>62 (24.1%)</v>
       </c>
       <c r="AB125" t="str">
-        <f t="shared" ref="AB125:AF125" si="27">CONCATENATE(S125," (",TEXT(S148,"0.0%"),")")</f>
+        <f t="shared" ref="AB125:AF125" si="28">CONCATENATE(S125," (",TEXT(S148,"0.0%"),")")</f>
         <v>29 (24.2%)</v>
       </c>
       <c r="AC125" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>76 (27.5%)</v>
       </c>
       <c r="AD125" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>36 (24.5%)</v>
       </c>
       <c r="AE125" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>13 (16.3%)</v>
       </c>
       <c r="AF125" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1231 (78.5%)</v>
       </c>
     </row>
@@ -8172,23 +8172,23 @@
         <v>195 (75.9%)</v>
       </c>
       <c r="AB126" t="str">
-        <f t="shared" ref="AB126:AF126" si="28">CONCATENATE(S126," (",TEXT(S149,"0.0%"),")")</f>
+        <f t="shared" ref="AB126:AF126" si="29">CONCATENATE(S126," (",TEXT(S149,"0.0%"),")")</f>
         <v>91 (75.8%)</v>
       </c>
       <c r="AC126" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>200 (72.5%)</v>
       </c>
       <c r="AD126" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>111 (75.5%)</v>
       </c>
       <c r="AE126" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>67 (83.8%)</v>
       </c>
       <c r="AF126" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>337 (21.5%)</v>
       </c>
     </row>
@@ -9366,23 +9366,23 @@
         <v>0.24124513618677043</v>
       </c>
       <c r="S148">
-        <f t="shared" ref="S148:W148" si="29">S125/S$127</f>
+        <f t="shared" ref="S148:W148" si="30">S125/S$127</f>
         <v>0.24166666666666667</v>
       </c>
       <c r="T148">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.27536231884057971</v>
       </c>
       <c r="U148">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.24489795918367346</v>
       </c>
       <c r="V148">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.16250000000000001</v>
       </c>
       <c r="W148">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.78507653061224492</v>
       </c>
     </row>
@@ -9433,27 +9433,27 @@
         <v>45</v>
       </c>
       <c r="R149">
-        <f t="shared" ref="R149:W149" si="30">R126/R$127</f>
+        <f t="shared" ref="R149:W149" si="31">R126/R$127</f>
         <v>0.75875486381322954</v>
       </c>
       <c r="S149">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.7583333333333333</v>
       </c>
       <c r="T149">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.72463768115942029</v>
       </c>
       <c r="U149">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.75510204081632648</v>
       </c>
       <c r="V149">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.83750000000000002</v>
       </c>
       <c r="W149">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.21492346938775511</v>
       </c>
     </row>

</xml_diff>